<commit_message>
DL Ngoc Hoan + DL VietGlobal
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang6/2.XulyBH/XLBH2206_DLNgocHoan.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang6/2.XulyBH/XLBH2206_DLNgocHoan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4035" windowWidth="10320" windowHeight="4065"/>
+    <workbookView xWindow="-15" yWindow="4035" windowWidth="10320" windowHeight="4065" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="VNSH02" sheetId="44" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="147">
   <si>
     <t>STT</t>
   </si>
@@ -339,9 +339,6 @@
     <t>Module GSM có dấu hiệu bị oxi hóa</t>
   </si>
   <si>
-    <t>Thay module GSM/GPS</t>
-  </si>
-  <si>
     <t>125.212.203.114,15959</t>
   </si>
   <si>
@@ -469,6 +466,30 @@
   </si>
   <si>
     <t>V3.3.21.3_R21111601</t>
+  </si>
+  <si>
+    <t>Thay module GSM/GPS (Khách báo không sửa chữa)</t>
+  </si>
+  <si>
+    <t>Mạch oxi hóa</t>
+  </si>
+  <si>
+    <t>Lỗi ống kính camera</t>
+  </si>
+  <si>
+    <t>Thiết bị bắt sóng có vấn đề</t>
+  </si>
+  <si>
+    <t>Cầu chì bị đứt, WP21120135S01463</t>
+  </si>
+  <si>
+    <t>Anh thông đang giữ, WP21120135S01459</t>
+  </si>
+  <si>
+    <t>WP21120135S01438</t>
+  </si>
+  <si>
+    <t>WP21120135S01398</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1450,9 @@
       <c r="B6" s="54">
         <v>44742</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="54">
+        <v>44759</v>
+      </c>
       <c r="D6" s="37" t="s">
         <v>64</v>
       </c>
@@ -1442,17 +1465,31 @@
       <c r="G6" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="37"/>
+      <c r="H6" s="37" t="s">
+        <v>143</v>
+      </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="59"/>
+      <c r="J6" s="39" t="s">
+        <v>102</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
+      <c r="M6" s="39" t="s">
+        <v>135</v>
+      </c>
       <c r="N6" s="1"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="O6" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="S6" s="3"/>
       <c r="T6" s="58"/>
       <c r="U6" s="72" t="s">
@@ -1470,7 +1507,9 @@
       <c r="B7" s="54">
         <v>44742</v>
       </c>
-      <c r="C7" s="54"/>
+      <c r="C7" s="54">
+        <v>44759</v>
+      </c>
       <c r="D7" s="37" t="s">
         <v>64</v>
       </c>
@@ -1482,11 +1521,11 @@
         <v>63</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K7" s="55"/>
       <c r="L7" s="39"/>
@@ -1521,7 +1560,9 @@
       <c r="B8" s="54">
         <v>44742</v>
       </c>
-      <c r="C8" s="54"/>
+      <c r="C8" s="54">
+        <v>44759</v>
+      </c>
       <c r="D8" s="37" t="s">
         <v>64</v>
       </c>
@@ -1532,17 +1573,31 @@
       <c r="G8" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="37"/>
+      <c r="H8" s="37" t="s">
+        <v>144</v>
+      </c>
       <c r="I8" s="51"/>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="K8" s="55"/>
       <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
+      <c r="M8" s="39" t="s">
+        <v>135</v>
+      </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="2"/>
+      <c r="O8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="P8" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="S8" s="3"/>
       <c r="T8" s="58"/>
       <c r="U8" s="73"/>
@@ -1558,7 +1613,9 @@
       <c r="B9" s="54">
         <v>44742</v>
       </c>
-      <c r="C9" s="54"/>
+      <c r="C9" s="54">
+        <v>44759</v>
+      </c>
       <c r="D9" s="37" t="s">
         <v>64</v>
       </c>
@@ -1569,19 +1626,33 @@
       <c r="G9" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="37"/>
+      <c r="H9" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="I9" s="51"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="K9" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
+      <c r="M9" s="39" t="s">
+        <v>135</v>
+      </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="2"/>
+      <c r="O9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="P9" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="S9" s="3"/>
       <c r="T9" s="58"/>
       <c r="U9" s="73"/>
@@ -1597,7 +1668,9 @@
       <c r="B10" s="54">
         <v>44742</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="54">
+        <v>44759</v>
+      </c>
       <c r="D10" s="37" t="s">
         <v>64</v>
       </c>
@@ -1608,23 +1681,25 @@
       <c r="G10" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="37"/>
+      <c r="H10" s="51" t="s">
+        <v>146</v>
+      </c>
       <c r="I10" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L10" s="39"/>
       <c r="M10" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P10" s="39" t="s">
         <v>83</v>
@@ -1963,7 +2038,7 @@
       </c>
       <c r="V21" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="W21" s="13"/>
     </row>
@@ -2208,7 +2283,7 @@
       </c>
       <c r="V29" s="9">
         <f>COUNTIF($R$6:$R$51,"*NG*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W29" s="13"/>
     </row>
@@ -2272,7 +2347,7 @@
       </c>
       <c r="V31" s="9">
         <f>COUNTIF($R$6:$R$51,"*LK*")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W31" s="13"/>
     </row>
@@ -2464,7 +2539,7 @@
       </c>
       <c r="V37" s="9">
         <f>SUM(V26:V36)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="W37" s="13"/>
     </row>
@@ -2550,7 +2625,7 @@
       </c>
       <c r="V40" s="9">
         <f>COUNTIF($O$6:$O$51,"*DM*")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W40" s="13"/>
     </row>
@@ -3558,7 +3633,7 @@
   <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C7" sqref="C7:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3773,7 +3848,9 @@
       <c r="B6" s="54">
         <v>44742</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="54">
+        <v>44759</v>
+      </c>
       <c r="D6" s="37" t="s">
         <v>67</v>
       </c>
@@ -3793,12 +3870,22 @@
         <v>77</v>
       </c>
       <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
+      <c r="M6" s="39" t="s">
+        <v>110</v>
+      </c>
       <c r="N6" s="1"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="O6" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="S6" s="3"/>
       <c r="T6" s="61"/>
       <c r="U6" s="72" t="s">
@@ -4213,7 +4300,7 @@
       </c>
       <c r="V20" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PM")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="13"/>
     </row>
@@ -4714,7 +4801,7 @@
       </c>
       <c r="V36" s="9">
         <f>COUNTIF($R$6:$R$51,"*KL*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W36" s="13"/>
     </row>
@@ -4746,7 +4833,7 @@
       </c>
       <c r="V37" s="9">
         <f>SUM(V26:V36)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W37" s="13"/>
     </row>
@@ -5839,8 +5926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6055,7 +6142,9 @@
       <c r="B6" s="54">
         <v>44742</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="54">
+        <v>44759</v>
+      </c>
       <c r="D6" s="37" t="s">
         <v>45</v>
       </c>
@@ -6068,14 +6157,14 @@
       </c>
       <c r="H6" s="37"/>
       <c r="I6" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J6" s="59"/>
       <c r="K6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M6" s="39" t="s">
         <v>38</v>
@@ -6110,7 +6199,9 @@
       <c r="B7" s="54">
         <v>44742</v>
       </c>
-      <c r="C7" s="54"/>
+      <c r="C7" s="54">
+        <v>44759</v>
+      </c>
       <c r="D7" s="37" t="s">
         <v>45</v>
       </c>
@@ -6123,14 +6214,14 @@
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J7" s="59"/>
       <c r="K7" s="55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L7" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M7" s="39" t="s">
         <v>38</v>
@@ -6163,7 +6254,9 @@
       <c r="B8" s="54">
         <v>44742</v>
       </c>
-      <c r="C8" s="54"/>
+      <c r="C8" s="54">
+        <v>44759</v>
+      </c>
       <c r="D8" s="37" t="s">
         <v>45</v>
       </c>
@@ -6176,17 +6269,17 @@
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L8" s="39"/>
       <c r="M8" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="s">
@@ -6216,7 +6309,9 @@
       <c r="B9" s="54">
         <v>44742</v>
       </c>
-      <c r="C9" s="54"/>
+      <c r="C9" s="54">
+        <v>44759</v>
+      </c>
       <c r="D9" s="37" t="s">
         <v>45</v>
       </c>
@@ -6233,13 +6328,13 @@
         <v>32</v>
       </c>
       <c r="K9" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L9" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M9" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
@@ -6269,7 +6364,9 @@
       <c r="B10" s="54">
         <v>44742</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="54">
+        <v>44759</v>
+      </c>
       <c r="D10" s="37" t="s">
         <v>45</v>
       </c>
@@ -6282,14 +6379,14 @@
       </c>
       <c r="H10" s="37"/>
       <c r="I10" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L10" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M10" s="39" t="s">
         <v>38</v>
@@ -8229,8 +8326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="K4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView showZeros="0" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8445,7 +8542,9 @@
       <c r="B6" s="54">
         <v>44742</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="54">
+        <v>44759</v>
+      </c>
       <c r="D6" s="37" t="s">
         <v>44</v>
       </c>
@@ -8458,11 +8557,11 @@
       </c>
       <c r="H6" s="37"/>
       <c r="I6" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J6" s="59"/>
       <c r="K6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L6" s="39" t="s">
         <v>77</v>
@@ -8500,7 +8599,9 @@
       <c r="B7" s="54">
         <v>44742</v>
       </c>
-      <c r="C7" s="54"/>
+      <c r="C7" s="54">
+        <v>44759</v>
+      </c>
       <c r="D7" s="37" t="s">
         <v>44</v>
       </c>
@@ -8513,17 +8614,17 @@
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K7" s="55"/>
       <c r="L7" s="39" t="s">
         <v>77</v>
       </c>
       <c r="M7" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1" t="s">
@@ -8553,7 +8654,9 @@
       <c r="B8" s="54">
         <v>44742</v>
       </c>
-      <c r="C8" s="54"/>
+      <c r="C8" s="54">
+        <v>44759</v>
+      </c>
       <c r="D8" s="37" t="s">
         <v>44</v>
       </c>
@@ -8568,7 +8671,7 @@
         <v>94</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="55" t="s">
@@ -8576,7 +8679,7 @@
       </c>
       <c r="L8" s="39"/>
       <c r="M8" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="s">
@@ -8606,7 +8709,9 @@
       <c r="B9" s="54">
         <v>44742</v>
       </c>
-      <c r="C9" s="54"/>
+      <c r="C9" s="54">
+        <v>44759</v>
+      </c>
       <c r="D9" s="37" t="s">
         <v>44</v>
       </c>
@@ -8621,7 +8726,7 @@
         <v>94</v>
       </c>
       <c r="I9" s="51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
@@ -8629,7 +8734,7 @@
       </c>
       <c r="L9" s="39"/>
       <c r="M9" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
@@ -8659,7 +8764,9 @@
       <c r="B10" s="54">
         <v>44742</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="54">
+        <v>44759</v>
+      </c>
       <c r="D10" s="37" t="s">
         <v>44</v>
       </c>
@@ -8674,7 +8781,7 @@
         <v>94</v>
       </c>
       <c r="I10" s="51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="24" t="s">
@@ -8714,7 +8821,9 @@
       <c r="B11" s="54">
         <v>44742</v>
       </c>
-      <c r="C11" s="54"/>
+      <c r="C11" s="54">
+        <v>44759</v>
+      </c>
       <c r="D11" s="37" t="s">
         <v>44</v>
       </c>
@@ -8728,14 +8837,14 @@
       <c r="H11" s="56"/>
       <c r="I11" s="51"/>
       <c r="J11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K11" s="38"/>
       <c r="L11" s="39" t="s">
         <v>77</v>
       </c>
       <c r="M11" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="s">
@@ -8765,7 +8874,9 @@
       <c r="B12" s="54">
         <v>44742</v>
       </c>
-      <c r="C12" s="54"/>
+      <c r="C12" s="54">
+        <v>44759</v>
+      </c>
       <c r="D12" s="37" t="s">
         <v>44</v>
       </c>
@@ -8780,19 +8891,19 @@
         <v>94</v>
       </c>
       <c r="I12" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L12" s="39" t="s">
         <v>77</v>
       </c>
       <c r="M12" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1" t="s">
@@ -8824,7 +8935,9 @@
       <c r="B13" s="54">
         <v>44742</v>
       </c>
-      <c r="C13" s="54"/>
+      <c r="C13" s="54">
+        <v>44759</v>
+      </c>
       <c r="D13" s="37" t="s">
         <v>44</v>
       </c>
@@ -8837,17 +8950,17 @@
       </c>
       <c r="H13" s="47"/>
       <c r="I13" s="51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="39" t="s">
         <v>77</v>
       </c>
       <c r="M13" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
@@ -8877,7 +8990,9 @@
       <c r="B14" s="54">
         <v>44742</v>
       </c>
-      <c r="C14" s="54"/>
+      <c r="C14" s="54">
+        <v>44759</v>
+      </c>
       <c r="D14" s="37" t="s">
         <v>44</v>
       </c>
@@ -8890,17 +9005,17 @@
       </c>
       <c r="H14" s="47"/>
       <c r="I14" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="39" t="s">
         <v>77</v>
       </c>
       <c r="M14" s="39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1" t="s">
@@ -8913,7 +9028,7 @@
         <v>18</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="61"/>
@@ -8930,7 +9045,9 @@
       <c r="B15" s="54">
         <v>44742</v>
       </c>
-      <c r="C15" s="54"/>
+      <c r="C15" s="54">
+        <v>44759</v>
+      </c>
       <c r="D15" s="37" t="s">
         <v>44</v>
       </c>
@@ -8953,12 +9070,12 @@
       </c>
       <c r="L15" s="39"/>
       <c r="M15" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="N15" s="63">
-        <v>375000</v>
-      </c>
-      <c r="O15" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="N15" s="63"/>
+      <c r="O15" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="P15" s="39" t="s">
         <v>83</v>
       </c>
@@ -8983,7 +9100,9 @@
       <c r="B16" s="54">
         <v>44742</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="54">
+        <v>44759</v>
+      </c>
       <c r="D16" s="37" t="s">
         <v>44</v>
       </c>
@@ -9040,7 +9159,9 @@
       <c r="B17" s="54">
         <v>44742</v>
       </c>
-      <c r="C17" s="54"/>
+      <c r="C17" s="54">
+        <v>44759</v>
+      </c>
       <c r="D17" s="37" t="s">
         <v>44</v>
       </c>
@@ -9093,7 +9214,9 @@
       <c r="B18" s="54">
         <v>44742</v>
       </c>
-      <c r="C18" s="54"/>
+      <c r="C18" s="54">
+        <v>44759</v>
+      </c>
       <c r="D18" s="37" t="s">
         <v>44</v>
       </c>
@@ -9106,17 +9229,17 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="39" t="s">
         <v>77</v>
       </c>
       <c r="M18" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1" t="s">
@@ -9144,7 +9267,9 @@
       <c r="B19" s="54">
         <v>44742</v>
       </c>
-      <c r="C19" s="54"/>
+      <c r="C19" s="54">
+        <v>44759</v>
+      </c>
       <c r="D19" s="37" t="s">
         <v>44</v>
       </c>
@@ -9159,11 +9284,11 @@
         <v>94</v>
       </c>
       <c r="I19" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L19" s="39" t="s">
         <v>77</v>
@@ -9201,7 +9326,9 @@
       <c r="B20" s="54">
         <v>44742</v>
       </c>
-      <c r="C20" s="54"/>
+      <c r="C20" s="54">
+        <v>44759</v>
+      </c>
       <c r="D20" s="37" t="s">
         <v>44</v>
       </c>
@@ -9216,11 +9343,11 @@
         <v>94</v>
       </c>
       <c r="I20" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L20" s="39" t="s">
         <v>77</v>
@@ -9259,7 +9386,9 @@
       <c r="B21" s="54">
         <v>44742</v>
       </c>
-      <c r="C21" s="54"/>
+      <c r="C21" s="54">
+        <v>44759</v>
+      </c>
       <c r="D21" s="37" t="s">
         <v>44</v>
       </c>
@@ -9272,15 +9401,27 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="51"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
+      <c r="M21" s="39" t="s">
+        <v>120</v>
+      </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="2"/>
+      <c r="O21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P21" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="S21" s="3"/>
       <c r="T21" s="13"/>
       <c r="U21" s="9" t="s">
@@ -9288,7 +9429,7 @@
       </c>
       <c r="V21" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W21" s="13"/>
     </row>
@@ -9299,7 +9440,9 @@
       <c r="B22" s="54">
         <v>44742</v>
       </c>
-      <c r="C22" s="54"/>
+      <c r="C22" s="54">
+        <v>44759</v>
+      </c>
       <c r="D22" s="37" t="s">
         <v>44</v>
       </c>
@@ -9314,19 +9457,19 @@
         <v>94</v>
       </c>
       <c r="I22" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L22" s="39" t="s">
         <v>77</v>
       </c>
       <c r="M22" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1" t="s">
@@ -9359,7 +9502,9 @@
       <c r="B23" s="54">
         <v>44742</v>
       </c>
-      <c r="C23" s="54"/>
+      <c r="C23" s="54">
+        <v>44759</v>
+      </c>
       <c r="D23" s="37" t="s">
         <v>44</v>
       </c>
@@ -9372,17 +9517,17 @@
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="39" t="s">
         <v>77</v>
       </c>
       <c r="M23" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1" t="s">
@@ -9410,7 +9555,9 @@
       <c r="B24" s="54">
         <v>44742</v>
       </c>
-      <c r="C24" s="54"/>
+      <c r="C24" s="54">
+        <v>44759</v>
+      </c>
       <c r="D24" s="37" t="s">
         <v>44</v>
       </c>
@@ -9675,7 +9822,7 @@
       </c>
       <c r="V31" s="9">
         <f>COUNTIF($R$6:$R$51,"*LK*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W31" s="13"/>
     </row>
@@ -9867,7 +10014,7 @@
       </c>
       <c r="V37" s="9">
         <f>SUM(V26:V36)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="W37" s="13"/>
     </row>
@@ -9985,7 +10132,7 @@
       </c>
       <c r="V41" s="9">
         <f>COUNTIF($O$6:$O$51,"*KS*")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W41" s="13"/>
     </row>
@@ -10961,7 +11108,7 @@
   <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11176,7 +11323,9 @@
       <c r="B6" s="54">
         <v>44742</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="54">
+        <v>44759</v>
+      </c>
       <c r="D6" s="37" t="s">
         <v>68</v>
       </c>
@@ -11188,7 +11337,7 @@
         <v>66</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="39"/>
@@ -11227,7 +11376,9 @@
       <c r="B7" s="54">
         <v>44742</v>
       </c>
-      <c r="C7" s="54"/>
+      <c r="C7" s="54">
+        <v>44759</v>
+      </c>
       <c r="D7" s="37" t="s">
         <v>68</v>
       </c>
@@ -11241,12 +11392,12 @@
       <c r="H7" s="37"/>
       <c r="I7" s="10"/>
       <c r="J7" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K7" s="55"/>
       <c r="L7" s="39"/>
       <c r="M7" s="39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1" t="s">
@@ -11276,7 +11427,9 @@
       <c r="B8" s="54">
         <v>44742</v>
       </c>
-      <c r="C8" s="54"/>
+      <c r="C8" s="54">
+        <v>44759</v>
+      </c>
       <c r="D8" s="37" t="s">
         <v>68</v>
       </c>
@@ -11288,7 +11441,7 @@
         <v>66</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I8" s="51"/>
       <c r="J8" s="1"/>
@@ -11325,7 +11478,9 @@
       <c r="B9" s="54">
         <v>44742</v>
       </c>
-      <c r="C9" s="54"/>
+      <c r="C9" s="54">
+        <v>44759</v>
+      </c>
       <c r="D9" s="37" t="s">
         <v>68</v>
       </c>
@@ -11337,14 +11492,14 @@
         <v>66</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I9" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L9" s="39"/>
       <c r="M9" s="39" t="s">
@@ -13315,7 +13470,7 @@
   <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13530,7 +13685,9 @@
       <c r="B6" s="54">
         <v>44742</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="54">
+        <v>44759</v>
+      </c>
       <c r="D6" s="37" t="s">
         <v>57</v>
       </c>
@@ -13544,12 +13701,12 @@
       <c r="H6" s="37"/>
       <c r="I6" s="10"/>
       <c r="J6" s="39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="39"/>
       <c r="M6" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="39" t="s">
@@ -15604,8 +15761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15820,7 +15977,9 @@
       <c r="B6" s="54">
         <v>44742</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="54">
+        <v>44759</v>
+      </c>
       <c r="D6" s="37" t="s">
         <v>69</v>
       </c>
@@ -15833,19 +15992,19 @@
       </c>
       <c r="H6" s="37"/>
       <c r="I6" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="M6" s="39" t="s">
         <v>123</v>
-      </c>
-      <c r="M6" s="39" t="s">
-        <v>124</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="39" t="s">

</xml_diff>